<commit_message>
Minimal template for 100% InPort XML submission
</commit_message>
<xml_diff>
--- a/Master_Template.xlsx
+++ b/Master_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="9564"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="9564" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data Set" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="262">
   <si>
     <t>level</t>
   </si>
@@ -1150,7 +1150,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1255,6 +1255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -1540,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -3819,7 +3820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -4470,8 +4471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:G57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4929,31 +4930,49 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="52" t="s">
+        <v>52</v>
+      </c>
       <c r="B57" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="52" t="s">
+        <v>52</v>
+      </c>
       <c r="B58" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="52" t="s">
+        <v>52</v>
+      </c>
       <c r="B59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="52" t="s">
+        <v>52</v>
+      </c>
       <c r="B60" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="52" t="s">
+        <v>52</v>
+      </c>
       <c r="B61" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="52" t="s">
+        <v>52</v>
+      </c>
       <c r="B62" t="s">
         <v>260</v>
       </c>

</xml_diff>